<commit_message>
Today was a good day :ballon:
</commit_message>
<xml_diff>
--- a/assets/generated/MultiItems.xlsx
+++ b/assets/generated/MultiItems.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="23955" windowHeight="4695" tabRatio="366" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="20730" windowHeight="4695" tabRatio="366"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="224">
   <si>
     <t>Type Decl.</t>
   </si>
@@ -145,15 +145,6 @@
   </si>
   <si>
     <t>Trad. Count</t>
-  </si>
-  <si>
-    <t>12*** Detajet e vleres (kujdes e inseruar zero, ne XML eshte 0.0)</t>
-  </si>
-  <si>
-    <t>General_information-&gt;Value_details</t>
-  </si>
-  <si>
-    <t>Value Det.</t>
   </si>
   <si>
     <t>13*** P.P.B (Bosh)</t>
@@ -494,9 +485,6 @@
   </si>
   <si>
     <t>4000</t>
-  </si>
-  <si>
-    <t>0+0+0+0-0</t>
   </si>
   <si>
     <t>1</t>
@@ -537,9 +525,6 @@
     <t>31</t>
   </si>
   <si>
-    <t>TR</t>
-  </si>
-  <si>
     <t>6516</t>
   </si>
   <si>
@@ -549,31 +534,12 @@
     <t>Ermal Nexhipi</t>
   </si>
   <si>
-    <t>6516.0</t>
-  </si>
-  <si>
-    <t>4110</t>
-  </si>
-  <si>
     <t>Property-&gt;Nbers-&gt;Total_number_of_packages(Nuk lexohet ketu)</t>
   </si>
   <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>Arka derrase</t>
-  </si>
-  <si>
     <t>- Me berthame celiku</t>
   </si>
   <si>
-    <t>PERCJELLES ALUMIMI I PERFORCUAR
-    ME CELIK ASCR 490/65 - 2000 M</t>
-  </si>
-  <si>
-    <t>3656</t>
-  </si>
-  <si>
     <t>Item-&gt;Valuation_item-&gt;Rate_of_adjustement</t>
   </si>
   <si>
@@ -583,19 +549,10 @@
     <t>Item-&gt;Valuation_item-&gt;Item_Invoice</t>
   </si>
   <si>
-    <t>MTLTR</t>
-  </si>
-  <si>
-    <t>76141000</t>
-  </si>
-  <si>
     <t>Item-&gt;Tarification-&gt;</t>
   </si>
   <si>
     <t>Attached_doc_item</t>
-  </si>
-  <si>
-    <t>862 863 380</t>
   </si>
   <si>
     <t>Item-&gt;Valuation_item-&gt;Gs_external_freight</t>
@@ -634,18 +591,12 @@
                 TIRANE</t>
   </si>
   <si>
-    <t>K71520008O</t>
-  </si>
-  <si>
     <t>IT</t>
   </si>
   <si>
     <t>KR</t>
   </si>
   <si>
-    <t>197366.0</t>
-  </si>
-  <si>
     <t>Korea Jugut</t>
   </si>
   <si>
@@ -668,6 +619,89 @@
   </si>
   <si>
     <t>AL140000</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Lidhje</t>
+  </si>
+  <si>
+    <t>GOMA TE REJA PER AUTOVETURA
+                ME R12-12 COPE
+    ME CELIK ASCR 490/65 - 2000 M</t>
+  </si>
+  <si>
+    <t>40111000</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>74.796</t>
+  </si>
+  <si>
+    <t>120.0</t>
+  </si>
+  <si>
+    <t>1618.0</t>
+  </si>
+  <si>
+    <t>1,618+0+0+0-0</t>
+  </si>
+  <si>
+    <t>- Goma autoveturash, te reja, 14 inch</t>
+  </si>
+  <si>
+    <t>GOMA TE REJA PER AUTOVETURA ME R14-88 COPE</t>
+  </si>
+  <si>
+    <t>16,605+0+0+0-0</t>
+  </si>
+  <si>
+    <t>Goma autoveturash, te reja, 15 inch</t>
+  </si>
+  <si>
+    <t>GOMA TE REJA FURGONASH
+                ME R15-90 COPE</t>
+  </si>
+  <si>
+    <t>20,622+0+0+0-0</t>
+  </si>
+  <si>
+    <t>Goma autoveturash, te reja, 16 inch</t>
+  </si>
+  <si>
+    <t>GOMA TE REJA AUTOVETURASH
+                ME R16- 87 COPE</t>
+  </si>
+  <si>
+    <t>23,453+0+0+0-0</t>
+  </si>
+  <si>
+    <t>Goma autoveturash, te reja, 17 inch</t>
+  </si>
+  <si>
+    <t>GOMA TE REJA AUTOVETURASH
+                ME R17- 78 COPE</t>
+  </si>
+  <si>
+    <t>26,284+0+0+0-0</t>
+  </si>
+  <si>
+    <t>74,536+0+0+0-0</t>
+  </si>
+  <si>
+    <t>L31616001H</t>
+  </si>
+  <si>
+    <t>Suppplementary_unit_code</t>
+  </si>
+  <si>
+    <t>Suppplementary_unit_quantity</t>
+  </si>
+  <si>
+    <t>C62</t>
   </si>
 </sst>
 </file>
@@ -794,7 +828,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -838,7 +872,12 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1167,10 +1206,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX4"/>
+  <dimension ref="A1:AW4"/>
   <sheetViews>
-    <sheetView topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="AX2" sqref="AX2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,57 +1231,56 @@
     <col min="15" max="15" width="23.140625" customWidth="1"/>
     <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.42578125" customWidth="1"/>
-    <col min="19" max="19" width="16.85546875" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.7109375" customWidth="1"/>
-    <col min="23" max="23" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.85546875" customWidth="1"/>
-    <col min="27" max="27" width="17.85546875" customWidth="1"/>
-    <col min="28" max="28" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.7109375" style="1" customWidth="1"/>
-    <col min="37" max="37" width="23.42578125" customWidth="1"/>
-    <col min="38" max="38" width="17" style="1" customWidth="1"/>
-    <col min="39" max="39" width="26.140625" style="1" customWidth="1"/>
-    <col min="40" max="40" width="15.42578125" customWidth="1"/>
-    <col min="41" max="41" width="18" customWidth="1"/>
-    <col min="42" max="42" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="17" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.7109375" customWidth="1"/>
+    <col min="22" max="22" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.85546875" customWidth="1"/>
+    <col min="26" max="26" width="17.85546875" customWidth="1"/>
+    <col min="27" max="27" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.7109375" style="1" customWidth="1"/>
+    <col min="36" max="36" width="23.42578125" customWidth="1"/>
+    <col min="37" max="37" width="17" style="1" customWidth="1"/>
+    <col min="38" max="38" width="26.140625" style="1" customWidth="1"/>
+    <col min="39" max="39" width="15.42578125" customWidth="1"/>
+    <col min="40" max="40" width="18" customWidth="1"/>
+    <col min="41" max="41" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="17" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:49" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="22"/>
+      <c r="E1" s="23"/>
       <c r="F1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="22"/>
+      <c r="H1" s="23"/>
       <c r="I1" s="2" t="s">
         <v>20</v>
       </c>
@@ -1255,10 +1293,10 @@
       <c r="L1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="24"/>
+      <c r="N1" s="25"/>
       <c r="O1" s="3" t="s">
         <v>36</v>
       </c>
@@ -1268,48 +1306,48 @@
       <c r="Q1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="T1" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="U1" s="19"/>
+      <c r="S1" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" s="20"/>
+      <c r="U1" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="V1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="2" t="s">
         <v>55</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="Y1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z1" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="2" t="s">
+      <c r="Y1" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB1" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="AC1" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="AH1" s="19"/>
-      <c r="AI1" s="14"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="AE1" s="20"/>
+      <c r="AF1" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="AG1" s="20"/>
+      <c r="AH1" s="14"/>
+      <c r="AI1" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="AJ1" s="3" t="s">
         <v>83</v>
       </c>
@@ -1317,46 +1355,43 @@
         <v>86</v>
       </c>
       <c r="AL1" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AM1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AN1" s="3" t="s">
-        <v>91</v>
-      </c>
       <c r="AO1" s="3" t="s">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="AP1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AR1" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="AR1" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="AS1" s="3" t="s">
         <v>141</v>
       </c>
       <c r="AT1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="AU1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="AV1" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AW1" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="AV1" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="AW1" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>148</v>
-      </c>
     </row>
-    <row r="2" spans="1:50" s="1" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" s="1" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
@@ -1388,7 +1423,7 @@
         <v>24</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>29</v>
@@ -1405,14 +1440,14 @@
       <c r="Q2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>44</v>
+      <c r="S2" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>53</v>
@@ -1421,34 +1456,34 @@
         <v>56</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>59</v>
+        <v>164</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>168</v>
+        <v>60</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>68</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>72</v>
       </c>
       <c r="AE2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG2" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="AH2" s="1" t="s">
         <v>78</v>
@@ -1459,20 +1494,17 @@
       <c r="AJ2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AK2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AX2" s="1" t="s">
-        <v>149</v>
+      <c r="AM2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="4" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:49" s="4" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
@@ -1521,11 +1553,11 @@
       <c r="Q3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="R3" s="4" t="s">
-        <v>45</v>
+      <c r="S3" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="U3" s="4" t="s">
         <v>51</v>
@@ -1537,195 +1569,189 @@
         <v>57</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>60</v>
+        <v>165</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>169</v>
+        <v>62</v>
       </c>
       <c r="Z3" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AA3" s="4" t="s">
         <v>66</v>
       </c>
       <c r="AB3" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AC3" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AD3" s="4" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="AE3" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="AF3" s="4" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="AG3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AH3" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AI3" s="4" t="s">
+      <c r="AI3" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AJ3" s="5" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="AK3" s="4" t="s">
-        <v>88</v>
-      </c>
+      <c r="AK3" s="5"/>
       <c r="AL3" s="5"/>
-      <c r="AM3" s="5"/>
-      <c r="AN3" s="4" t="s">
-        <v>73</v>
-      </c>
+      <c r="AM3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO3" s="5"/>
       <c r="AP3" s="5"/>
-      <c r="AQ3" s="5"/>
-      <c r="AS3" s="4" t="s">
-        <v>143</v>
-      </c>
+      <c r="AR3" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="AS3" s="5"/>
       <c r="AT3" s="5"/>
       <c r="AU3" s="5"/>
       <c r="AV3" s="5"/>
-      <c r="AW3" s="5"/>
-      <c r="AX3" s="4" t="s">
-        <v>150</v>
+      <c r="AW3" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:50" s="6" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" s="6" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B4" s="12">
         <v>4</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="G4" s="12">
         <v>1</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="T4" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="AB4" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="AC4" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="AD4" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="AE4" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="AF4" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="AG4" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="AH4" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="AI4" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="AJ4" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="U4" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="V4" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="W4" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="X4" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="Y4" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="Z4" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="AA4" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="AB4" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="AC4" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="AD4" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="AE4" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="AF4" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="AG4" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="AH4" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="AI4" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="AJ4" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="AK4" s="7" t="s">
-        <v>171</v>
-      </c>
+      <c r="AK4" s="7"/>
       <c r="AL4" s="7"/>
-      <c r="AM4" s="7"/>
-      <c r="AN4" s="6" t="s">
-        <v>213</v>
-      </c>
+      <c r="AM4" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="AO4" s="7"/>
       <c r="AP4" s="7"/>
-      <c r="AQ4" s="7"/>
-      <c r="AS4" s="6" t="s">
-        <v>174</v>
-      </c>
+      <c r="AR4" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="AS4" s="7"/>
       <c r="AT4" s="7"/>
       <c r="AU4" s="7"/>
       <c r="AV4" s="7"/>
-      <c r="AW4" s="7"/>
-      <c r="AX4" s="6" t="s">
-        <v>175</v>
+      <c r="AW4" s="6" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="S1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1734,10 +1760,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH4"/>
+  <dimension ref="A1:AJ24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AI4" sqref="AI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,31 +1785,33 @@
     <col min="29" max="29" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="12" customWidth="1"/>
     <col min="34" max="34" width="25.28515625" customWidth="1"/>
+    <col min="35" max="35" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="23" t="s">
+      <c r="G1" s="25"/>
+      <c r="H1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -1799,267 +1827,283 @@
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
       <c r="X1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y1" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="Y1" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z1" s="24"/>
+      <c r="Z1" s="25"/>
       <c r="AA1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD1" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="AB1" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="AE1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF1" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="19"/>
+      <c r="AF1" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="20"/>
     </row>
-    <row r="2" spans="1:34" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="V2" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="W2" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="T2" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="U2" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="V2" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="W2" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="Z2" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
       <c r="AD2" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>221</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="X3" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="V3" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="X3" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="Y3" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="Z3" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
       <c r="AC3" s="4"/>
       <c r="AD3" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="AE3" s="4"/>
       <c r="AF3" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AG3" s="4" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="AH3" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>221</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" s="17" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>160</v>
+        <v>198</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>177</v>
+        <v>203</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>173</v>
+        <v>204</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
+        <v>153</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>153</v>
+      </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
@@ -2067,31 +2111,389 @@
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
       <c r="X4" s="6" t="s">
-        <v>187</v>
+        <v>162</v>
       </c>
       <c r="Y4" s="6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Z4" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="AE4" s="6"/>
       <c r="AF4" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="AG4" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="AH4" s="17"/>
+        <v>206</v>
+      </c>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="18"/>
+      <c r="AI4" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="AJ4" s="17">
+        <v>50</v>
+      </c>
     </row>
+    <row r="5" spans="1:36" s="17" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>88</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="F5" s="17">
+        <v>40111000</v>
+      </c>
+      <c r="G5" s="17">
+        <v>400</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="I5" s="17">
+        <v>682.976</v>
+      </c>
+      <c r="J5" s="17">
+        <v>682.976</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="L5" s="17">
+        <v>1232</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="N5" s="17">
+        <v>135.29</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="X5" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y5" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD5" s="17">
+        <v>1232</v>
+      </c>
+      <c r="AF5" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="AI5" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="AJ5" s="17">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>90</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="F6" s="17">
+        <v>40111000</v>
+      </c>
+      <c r="G6" s="17">
+        <v>600</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="I6" s="17">
+        <v>1106.5360000000001</v>
+      </c>
+      <c r="J6" s="17">
+        <v>1106.5360000000001</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="L6" s="17">
+        <v>1740</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="N6" s="17">
+        <v>191.08</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="X6" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y6" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD6" s="17">
+        <v>1530</v>
+      </c>
+      <c r="AF6" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="AI6" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="AJ6" s="17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>87</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="F7" s="17">
+        <v>40111000</v>
+      </c>
+      <c r="G7" s="17">
+        <v>700</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="I7" s="17">
+        <v>1106.5360000000001</v>
+      </c>
+      <c r="J7" s="17">
+        <v>1106.5360000000001</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="L7" s="17">
+        <v>1740</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="N7" s="17">
+        <v>191.08</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y7" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z7" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD7" s="17">
+        <v>1740</v>
+      </c>
+      <c r="AF7" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="AI7" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="AJ7" s="17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
+        <v>78</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="F8" s="17">
+        <v>40111000</v>
+      </c>
+      <c r="G8" s="17">
+        <v>700</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="I8" s="17">
+        <v>1121.52</v>
+      </c>
+      <c r="J8" s="17">
+        <v>1121.52</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="L8" s="17">
+        <v>1950</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="N8" s="17">
+        <v>214.14</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="X8" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y8" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z8" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD8" s="17">
+        <v>1950</v>
+      </c>
+      <c r="AF8" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="AI8" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="AJ8" s="17">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" s="17" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
+        <v>28</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="F9" s="17">
+        <v>40111000</v>
+      </c>
+      <c r="G9" s="17">
+        <v>700</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="I9" s="17">
+        <v>366.8</v>
+      </c>
+      <c r="J9" s="17">
+        <v>366.8</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="L9" s="17">
+        <v>756</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="N9" s="17">
+        <v>83.02</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="X9" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y9" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z9" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD9" s="17">
+        <v>5530</v>
+      </c>
+      <c r="AF9" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="AI9" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="AJ9" s="17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:36" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:36" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:36" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:36" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:36" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:36" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="Y1:Z1"/>

</xml_diff>